<commit_message>
IC95 RR interpolations and plots
</commit_message>
<xml_diff>
--- a/data/RR_table_quanti.xlsx
+++ b/data/RR_table_quanti.xlsx
@@ -1,17 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inesmasurel/Library/Mobile Documents/com~apple~CloudDocs/Desktop/Pasteur-Cnam/Stage MS - ENS/DOUGLAS/DOUGLAS_model/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2431A3-9236-4E49-A1EA-A69E164CB583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Mid" sheetId="1" r:id="rId1"/>
+    <sheet name="Upper" sheetId="2" r:id="rId2"/>
+    <sheet name="Lower" sheetId="3" r:id="rId3"/>
+    <sheet name="Mid to upper lower" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
   <si>
     <t>food_group</t>
   </si>
@@ -61,38 +73,66 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF262626"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF262626"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,46 +140,62 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -329,64 +385,69 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.38"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C1" s="2">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="D1" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="E1" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="F1" s="2">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="G1" s="2">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="H1" s="2">
-        <v>250.0</v>
+        <v>250</v>
       </c>
       <c r="I1" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="J1" s="2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="K1" s="2">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="L1" s="2">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="M1" s="2">
-        <v>700.0</v>
+        <v>700</v>
       </c>
       <c r="N1" s="2">
-        <v>800.0</v>
+        <v>800</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -401,18 +462,18 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5">
         <v>1.05</v>
       </c>
       <c r="D2" s="5">
-        <v>1.09</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="E2" s="5">
         <v>1.18</v>
@@ -439,15 +500,15 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D3" s="5">
         <v>1.18</v>
@@ -477,47 +538,47 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="5">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="5">
-        <v>0.985</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="G5" s="5">
         <v>0.97</v>
@@ -529,24 +590,24 @@
         <v>0.99</v>
       </c>
       <c r="K5" s="5">
-        <v>1.015</v>
+        <v>1.0149999999999999</v>
       </c>
       <c r="L5" s="5">
         <v>1.04</v>
       </c>
       <c r="M5" s="5">
-        <v>1.065</v>
+        <v>1.0649999999999999</v>
       </c>
       <c r="N5" s="5">
-        <v>1.09</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5">
         <v>0.95</v>
@@ -573,12 +634,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5">
         <v>0.98</v>
@@ -593,12 +654,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="5">
         <v>0.97</v>
@@ -610,7 +671,7 @@
         <v>0.89</v>
       </c>
       <c r="F8" s="5">
-        <v>0.865</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="G8" s="5">
         <v>0.84</v>
@@ -637,12 +698,12 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5">
         <v>0.84</v>
@@ -657,15 +718,15 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5">
-        <v>0.965</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="D10" s="5">
         <v>0.93</v>
@@ -674,13 +735,13 @@
         <v>0.87</v>
       </c>
       <c r="F10" s="5">
-        <v>0.835</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="G10" s="5">
         <v>0.8</v>
       </c>
       <c r="H10" s="5">
-        <v>0.785</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="I10" s="5">
         <v>0.77</v>
@@ -701,12 +762,12 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="5">
         <v>0.9</v>
@@ -727,15 +788,15 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="5">
-        <v>0.935</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="D12" s="5">
         <v>0.87</v>
@@ -771,12 +832,12 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="5">
         <v>0.94</v>
@@ -788,10 +849,10 @@
         <v>1.03</v>
       </c>
       <c r="G13" s="5">
-        <v>1.09</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="H13" s="5">
-        <v>1.16</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="I13" s="5">
         <v>1.24</v>
@@ -803,41 +864,41 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="5">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5">
-        <v>1.0075</v>
+        <v>1.0075000000000001</v>
       </c>
       <c r="D15" s="5">
-        <v>1.015</v>
+        <v>1.0149999999999999</v>
       </c>
       <c r="E15" s="5">
         <v>1.03</v>
       </c>
       <c r="F15" s="5">
-        <v>1.045</v>
+        <v>1.0449999999999999</v>
       </c>
       <c r="G15" s="5">
         <v>1.06</v>
@@ -849,22 +910,1959 @@
         <v>1.08</v>
       </c>
       <c r="J15" s="5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K15" s="5">
-        <v>1.12</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="L15" s="5">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M15" s="5">
-        <v>1.16</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="N15" s="5">
         <v>1.18</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52511AF-CE91-C645-B98F-638F567A8977}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
+        <v>25</v>
+      </c>
+      <c r="D1" s="3">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3">
+        <v>100</v>
+      </c>
+      <c r="F1" s="3">
+        <v>150</v>
+      </c>
+      <c r="G1" s="3">
+        <v>200</v>
+      </c>
+      <c r="H1" s="3">
+        <v>250</v>
+      </c>
+      <c r="I1" s="3">
+        <v>300</v>
+      </c>
+      <c r="J1" s="3">
+        <v>400</v>
+      </c>
+      <c r="K1" s="3">
+        <v>500</v>
+      </c>
+      <c r="L1" s="3">
+        <v>600</v>
+      </c>
+      <c r="M1" s="3">
+        <v>700</v>
+      </c>
+      <c r="N1" s="3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <f>Mid!B2+'Mid to upper lower'!B2</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <f>Mid!C2+'Mid to upper lower'!C2</f>
+        <v>1.0549999999999999</v>
+      </c>
+      <c r="D2" s="6">
+        <f>Mid!D2+'Mid to upper lower'!D2</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E2" s="6">
+        <f>Mid!E2+'Mid to upper lower'!E2</f>
+        <v>1.2</v>
+      </c>
+      <c r="F2" s="6">
+        <f>Mid!F2+'Mid to upper lower'!F2</f>
+        <v>1.335</v>
+      </c>
+      <c r="G2" s="6">
+        <f>Mid!G2+'Mid to upper lower'!G2</f>
+        <v>1.47</v>
+      </c>
+      <c r="H2" s="6">
+        <f>Mid!H2+'Mid to upper lower'!H2</f>
+        <v>1.61</v>
+      </c>
+      <c r="I2" s="6">
+        <f>Mid!I2+'Mid to upper lower'!I2</f>
+        <v>1.7799999999999998</v>
+      </c>
+      <c r="J2" s="6">
+        <f>Mid!J2+'Mid to upper lower'!J2</f>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="K2" s="6">
+        <f>Mid!K2+'Mid to upper lower'!K2</f>
+        <v>2.3600000000000003</v>
+      </c>
+      <c r="L2" s="6">
+        <f>Mid!L2+'Mid to upper lower'!L2</f>
+        <v>2.6799999999999997</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <f>Mid!B3+'Mid to upper lower'!B3</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <f>Mid!C3+'Mid to upper lower'!C3</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D3" s="6">
+        <f>Mid!D3+'Mid to upper lower'!D3</f>
+        <v>1.2</v>
+      </c>
+      <c r="E3" s="6">
+        <f>Mid!E3+'Mid to upper lower'!E3</f>
+        <v>1.35</v>
+      </c>
+      <c r="F3" s="6">
+        <f>Mid!F3+'Mid to upper lower'!F3</f>
+        <v>1.53</v>
+      </c>
+      <c r="G3" s="6">
+        <f>Mid!G3+'Mid to upper lower'!G3</f>
+        <v>1.72</v>
+      </c>
+      <c r="H3" s="6">
+        <f>Mid!H3+'Mid to upper lower'!H3</f>
+        <v>1.91</v>
+      </c>
+      <c r="I3" s="6">
+        <f>Mid!I3+'Mid to upper lower'!I3</f>
+        <v>2.1</v>
+      </c>
+      <c r="J3" s="6">
+        <f>Mid!J3+'Mid to upper lower'!J3</f>
+        <v>2.4499999999999997</v>
+      </c>
+      <c r="K3" s="6">
+        <f>Mid!K3+'Mid to upper lower'!K3</f>
+        <v>2.81</v>
+      </c>
+      <c r="L3" s="6">
+        <f>Mid!L3+'Mid to upper lower'!L3</f>
+        <v>3.19</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <f>Mid!B4+'Mid to upper lower'!B4</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <f>Mid!C4+'Mid to upper lower'!C4</f>
+        <v>1.05</v>
+      </c>
+      <c r="D4" s="6">
+        <f>Mid!D4+'Mid to upper lower'!D4</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E4" s="6">
+        <f>Mid!E4+'Mid to upper lower'!E4</f>
+        <v>1.2</v>
+      </c>
+      <c r="F4" s="6">
+        <f>Mid!F4+'Mid to upper lower'!F4</f>
+        <v>1.25</v>
+      </c>
+      <c r="G4" s="6">
+        <f>Mid!G4+'Mid to upper lower'!G4</f>
+        <v>1.3</v>
+      </c>
+      <c r="H4" s="6">
+        <f>Mid!H4+'Mid to upper lower'!H4</f>
+        <v>1.35</v>
+      </c>
+      <c r="I4" s="6">
+        <f>Mid!I4+'Mid to upper lower'!I4</f>
+        <v>1.4</v>
+      </c>
+      <c r="J4" s="6">
+        <f>Mid!J4+'Mid to upper lower'!J4</f>
+        <v>1.45</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6">
+        <f>Mid!E5+'Mid to upper lower'!E5</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6">
+        <f>Mid!G5+'Mid to upper lower'!G5</f>
+        <v>0.99</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6">
+        <f>Mid!I5+'Mid to upper lower'!I5</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="6">
+        <f>Mid!J5+'Mid to upper lower'!J5</f>
+        <v>1.01</v>
+      </c>
+      <c r="K5" s="6">
+        <f>Mid!K5+'Mid to upper lower'!K5</f>
+        <v>1.0399999999999998</v>
+      </c>
+      <c r="L5" s="6">
+        <f>Mid!L5+'Mid to upper lower'!L5</f>
+        <v>1.07</v>
+      </c>
+      <c r="M5" s="6">
+        <f>Mid!M5+'Mid to upper lower'!M5</f>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="N5" s="6">
+        <f>Mid!N5+'Mid to upper lower'!N5</f>
+        <v>1.1300000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6">
+        <f>Mid!D6+'Mid to upper lower'!D6</f>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="E6" s="6">
+        <f>Mid!E6+'Mid to upper lower'!E6</f>
+        <v>0.96000000000000008</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6">
+        <f>Mid!G6+'Mid to upper lower'!G6</f>
+        <v>0.96</v>
+      </c>
+      <c r="H6" s="6">
+        <f>Mid!H6+'Mid to upper lower'!H6</f>
+        <v>0.96</v>
+      </c>
+      <c r="I6" s="6">
+        <f>Mid!I6+'Mid to upper lower'!I6</f>
+        <v>0.98</v>
+      </c>
+      <c r="J6" s="6">
+        <f>Mid!J6+'Mid to upper lower'!J6</f>
+        <v>1.02</v>
+      </c>
+      <c r="K6" s="6">
+        <f>Mid!K6+'Mid to upper lower'!K6</f>
+        <v>1.08</v>
+      </c>
+      <c r="L6" s="6">
+        <f>Mid!L6+'Mid to upper lower'!L6</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6">
+        <f>Mid!C7+'Mid to upper lower'!C7</f>
+        <v>1.04</v>
+      </c>
+      <c r="D7" s="6">
+        <f>Mid!D7+'Mid to upper lower'!D7</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E7" s="6">
+        <f>Mid!E7+'Mid to upper lower'!E7</f>
+        <v>1.37</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6">
+        <f>Mid!G7+'Mid to upper lower'!G7</f>
+        <v>1.65</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <f>Mid!B8+'Mid to upper lower'!B8</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <f>Mid!C8+'Mid to upper lower'!C8</f>
+        <v>0.97</v>
+      </c>
+      <c r="D8" s="6">
+        <f>Mid!D8+'Mid to upper lower'!D8</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="E8" s="6">
+        <f>Mid!E8+'Mid to upper lower'!E8</f>
+        <v>0.9</v>
+      </c>
+      <c r="F8" s="6">
+        <f>Mid!F8+'Mid to upper lower'!F8</f>
+        <v>0.88</v>
+      </c>
+      <c r="G8" s="6">
+        <f>Mid!G8+'Mid to upper lower'!G8</f>
+        <v>0.86</v>
+      </c>
+      <c r="H8" s="6">
+        <f>Mid!H8+'Mid to upper lower'!H8</f>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="I8" s="6">
+        <f>Mid!I8+'Mid to upper lower'!I8</f>
+        <v>0.85</v>
+      </c>
+      <c r="J8" s="6">
+        <f>Mid!J8+'Mid to upper lower'!J8</f>
+        <v>0.84500000000000008</v>
+      </c>
+      <c r="K8" s="6">
+        <f>Mid!K8+'Mid to upper lower'!K8</f>
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="L8" s="6">
+        <f>Mid!L8+'Mid to upper lower'!L8</f>
+        <v>0.8600000000000001</v>
+      </c>
+      <c r="M8" s="6">
+        <f>Mid!M8+'Mid to upper lower'!M8</f>
+        <v>0.87999999999999989</v>
+      </c>
+      <c r="N8" s="6">
+        <f>Mid!N8+'Mid to upper lower'!N8</f>
+        <v>0.90999999999999992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6">
+        <f>Mid!C9+'Mid to upper lower'!C9</f>
+        <v>0.86</v>
+      </c>
+      <c r="D9" s="6">
+        <f>Mid!D9+'Mid to upper lower'!D9</f>
+        <v>0.9</v>
+      </c>
+      <c r="E9" s="6">
+        <f>Mid!E9+'Mid to upper lower'!E9</f>
+        <v>0.98</v>
+      </c>
+      <c r="F9" s="6">
+        <f>Mid!F9+'Mid to upper lower'!F9</f>
+        <v>1.0699999999999998</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6">
+        <f>Mid!D10+'Mid to upper lower'!D10</f>
+        <v>0.94500000000000006</v>
+      </c>
+      <c r="E10" s="6">
+        <f>Mid!E10+'Mid to upper lower'!E10</f>
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="F10" s="6">
+        <f>Mid!F10+'Mid to upper lower'!F10</f>
+        <v>0.875</v>
+      </c>
+      <c r="G10" s="6">
+        <f>Mid!G10+'Mid to upper lower'!G10</f>
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="H10" s="6">
+        <f>Mid!H10+'Mid to upper lower'!H10</f>
+        <v>0.83500000000000008</v>
+      </c>
+      <c r="I10" s="6">
+        <f>Mid!I10+'Mid to upper lower'!I10</f>
+        <v>0.82000000000000006</v>
+      </c>
+      <c r="J10" s="6">
+        <f>Mid!J10+'Mid to upper lower'!J10</f>
+        <v>0.81</v>
+      </c>
+      <c r="K10" s="6">
+        <f>Mid!K10+'Mid to upper lower'!K10</f>
+        <v>0.81</v>
+      </c>
+      <c r="L10" s="6">
+        <f>Mid!L10+'Mid to upper lower'!L10</f>
+        <v>0.81</v>
+      </c>
+      <c r="M10" s="6">
+        <f>Mid!M10+'Mid to upper lower'!M10</f>
+        <v>0.82000000000000006</v>
+      </c>
+      <c r="N10" s="6">
+        <f>Mid!N10+'Mid to upper lower'!N10</f>
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6">
+        <f>Mid!C11+'Mid to upper lower'!C11</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6">
+        <f>Mid!E11+'Mid to upper lower'!E11</f>
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6">
+        <f>Mid!G11+'Mid to upper lower'!G11</f>
+        <v>0.9</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
+        <f>Mid!I11+'Mid to upper lower'!I11</f>
+        <v>0.9</v>
+      </c>
+      <c r="J11" s="6">
+        <f>Mid!J11+'Mid to upper lower'!J11</f>
+        <v>0.91999999999999993</v>
+      </c>
+      <c r="K11" s="6">
+        <f>Mid!K11+'Mid to upper lower'!K11</f>
+        <v>0.96</v>
+      </c>
+      <c r="L11" s="6">
+        <f>Mid!L11+'Mid to upper lower'!L11</f>
+        <v>1.02</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6">
+        <f>Mid!D12+'Mid to upper lower'!D12</f>
+        <v>0.88</v>
+      </c>
+      <c r="E12" s="6">
+        <f>Mid!E12+'Mid to upper lower'!E12</f>
+        <v>0.82000000000000006</v>
+      </c>
+      <c r="F12" s="6">
+        <f>Mid!F12+'Mid to upper lower'!F12</f>
+        <v>0.79</v>
+      </c>
+      <c r="G12" s="6">
+        <f>Mid!G12+'Mid to upper lower'!G12</f>
+        <v>0.76</v>
+      </c>
+      <c r="H12" s="6">
+        <f>Mid!H12+'Mid to upper lower'!H12</f>
+        <v>0.75</v>
+      </c>
+      <c r="I12" s="6">
+        <f>Mid!I12+'Mid to upper lower'!I12</f>
+        <v>0.76</v>
+      </c>
+      <c r="J12" s="6">
+        <f>Mid!J12+'Mid to upper lower'!J12</f>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="K12" s="6">
+        <f>Mid!K12+'Mid to upper lower'!K12</f>
+        <v>0.82</v>
+      </c>
+      <c r="L12" s="6">
+        <f>Mid!L12+'Mid to upper lower'!L12</f>
+        <v>0.92</v>
+      </c>
+      <c r="M12" s="6">
+        <f>Mid!M12+'Mid to upper lower'!M12</f>
+        <v>0.94000000000000006</v>
+      </c>
+      <c r="N12" s="6">
+        <f>Mid!N12+'Mid to upper lower'!N12</f>
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6">
+        <f>Mid!D13+'Mid to upper lower'!D13</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
+        <f>Mid!E13+'Mid to upper lower'!E13</f>
+        <v>1.05</v>
+      </c>
+      <c r="F13" s="6">
+        <f>Mid!F13+'Mid to upper lower'!F13</f>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="G13" s="6">
+        <f>Mid!G13+'Mid to upper lower'!G13</f>
+        <v>1.2200000000000002</v>
+      </c>
+      <c r="H13" s="6">
+        <f>Mid!H13+'Mid to upper lower'!H13</f>
+        <v>1.3199999999999998</v>
+      </c>
+      <c r="I13" s="6">
+        <f>Mid!I13+'Mid to upper lower'!I13</f>
+        <v>1.43</v>
+      </c>
+      <c r="J13" s="6">
+        <f>Mid!J13+'Mid to upper lower'!J13</f>
+        <v>1.65</v>
+      </c>
+      <c r="K13" s="6">
+        <f>Mid!K13+'Mid to upper lower'!K13</f>
+        <v>1.8800000000000001</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <f>Mid!B14+'Mid to upper lower'!B14</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
+        <f>Mid!C14+'Mid to upper lower'!C14</f>
+        <v>1.05</v>
+      </c>
+      <c r="D14" s="6">
+        <f>Mid!D14+'Mid to upper lower'!D14</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E14" s="6">
+        <f>Mid!E14+'Mid to upper lower'!E14</f>
+        <v>1.2</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <f>Mid!B15+'Mid to upper lower'!B15</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="6">
+        <f>Mid!C15+'Mid to upper lower'!C15</f>
+        <v>1.02</v>
+      </c>
+      <c r="D15" s="6">
+        <f>Mid!D15+'Mid to upper lower'!D15</f>
+        <v>1.0399999999999998</v>
+      </c>
+      <c r="E15" s="6">
+        <f>Mid!E15+'Mid to upper lower'!E15</f>
+        <v>1.08</v>
+      </c>
+      <c r="F15" s="6">
+        <f>Mid!F15+'Mid to upper lower'!F15</f>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="G15" s="6">
+        <f>Mid!G15+'Mid to upper lower'!G15</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H15" s="6">
+        <f>Mid!H15+'Mid to upper lower'!H15</f>
+        <v>1.135</v>
+      </c>
+      <c r="I15" s="6">
+        <f>Mid!I15+'Mid to upper lower'!I15</f>
+        <v>1.1500000000000001</v>
+      </c>
+      <c r="J15" s="6">
+        <f>Mid!J15+'Mid to upper lower'!J15</f>
+        <v>1.1800000000000002</v>
+      </c>
+      <c r="K15" s="6">
+        <f>Mid!K15+'Mid to upper lower'!K15</f>
+        <v>1.2100000000000002</v>
+      </c>
+      <c r="L15" s="6">
+        <f>Mid!L15+'Mid to upper lower'!L15</f>
+        <v>1.24</v>
+      </c>
+      <c r="M15" s="6">
+        <f>Mid!M15+'Mid to upper lower'!M15</f>
+        <v>1.27</v>
+      </c>
+      <c r="N15" s="6">
+        <f>Mid!N15+'Mid to upper lower'!N15</f>
+        <v>1.3199999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A723EE2E-8835-E04A-880B-B880DB74E2B3}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
+        <v>25</v>
+      </c>
+      <c r="D1" s="3">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3">
+        <v>100</v>
+      </c>
+      <c r="F1" s="3">
+        <v>150</v>
+      </c>
+      <c r="G1" s="3">
+        <v>200</v>
+      </c>
+      <c r="H1" s="3">
+        <v>250</v>
+      </c>
+      <c r="I1" s="3">
+        <v>300</v>
+      </c>
+      <c r="J1" s="3">
+        <v>400</v>
+      </c>
+      <c r="K1" s="3">
+        <v>500</v>
+      </c>
+      <c r="L1" s="3">
+        <v>600</v>
+      </c>
+      <c r="M1" s="3">
+        <v>700</v>
+      </c>
+      <c r="N1" s="3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <f>Mid!B2-'Mid to upper lower'!B2</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <f>Mid!C2-'Mid to upper lower'!C2</f>
+        <v>1.0450000000000002</v>
+      </c>
+      <c r="D2" s="6">
+        <f>Mid!D2-'Mid to upper lower'!D2</f>
+        <v>1.08</v>
+      </c>
+      <c r="E2" s="6">
+        <f>Mid!E2-'Mid to upper lower'!E2</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F2" s="6">
+        <f>Mid!F2-'Mid to upper lower'!F2</f>
+        <v>1.2650000000000001</v>
+      </c>
+      <c r="G2" s="6">
+        <f>Mid!G2-'Mid to upper lower'!G2</f>
+        <v>1.3699999999999999</v>
+      </c>
+      <c r="H2" s="6">
+        <f>Mid!H2-'Mid to upper lower'!H2</f>
+        <v>1.47</v>
+      </c>
+      <c r="I2" s="6">
+        <f>Mid!I2-'Mid to upper lower'!I2</f>
+        <v>1.54</v>
+      </c>
+      <c r="J2" s="6">
+        <f>Mid!J2-'Mid to upper lower'!J2</f>
+        <v>1.73</v>
+      </c>
+      <c r="K2" s="6">
+        <f>Mid!K2-'Mid to upper lower'!K2</f>
+        <v>1.9200000000000002</v>
+      </c>
+      <c r="L2" s="6">
+        <f>Mid!L2-'Mid to upper lower'!L2</f>
+        <v>2.08</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <f>Mid!B3-'Mid to upper lower'!B3</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <f>Mid!C3-'Mid to upper lower'!C3</f>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D3" s="6">
+        <f>Mid!D3-'Mid to upper lower'!D3</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E3" s="6">
+        <f>Mid!E3-'Mid to upper lower'!E3</f>
+        <v>1.25</v>
+      </c>
+      <c r="F3" s="6">
+        <f>Mid!F3-'Mid to upper lower'!F3</f>
+        <v>1.3299999999999998</v>
+      </c>
+      <c r="G3" s="6">
+        <f>Mid!G3-'Mid to upper lower'!G3</f>
+        <v>1.4200000000000002</v>
+      </c>
+      <c r="H3" s="6">
+        <f>Mid!H3-'Mid to upper lower'!H3</f>
+        <v>1.51</v>
+      </c>
+      <c r="I3" s="6">
+        <f>Mid!I3-'Mid to upper lower'!I3</f>
+        <v>1.6</v>
+      </c>
+      <c r="J3" s="6">
+        <f>Mid!J3-'Mid to upper lower'!J3</f>
+        <v>1.8099999999999998</v>
+      </c>
+      <c r="K3" s="6">
+        <f>Mid!K3-'Mid to upper lower'!K3</f>
+        <v>2.0100000000000002</v>
+      </c>
+      <c r="L3" s="6">
+        <f>Mid!L3-'Mid to upper lower'!L3</f>
+        <v>2.19</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <f>Mid!B4-'Mid to upper lower'!B4</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <f>Mid!C4-'Mid to upper lower'!C4</f>
+        <v>0.95</v>
+      </c>
+      <c r="D4" s="6">
+        <f>Mid!D4-'Mid to upper lower'!D4</f>
+        <v>0.9</v>
+      </c>
+      <c r="E4" s="6">
+        <f>Mid!E4-'Mid to upper lower'!E4</f>
+        <v>0.8</v>
+      </c>
+      <c r="F4" s="6">
+        <f>Mid!F4-'Mid to upper lower'!F4</f>
+        <v>0.75</v>
+      </c>
+      <c r="G4" s="6">
+        <f>Mid!G4-'Mid to upper lower'!G4</f>
+        <v>0.7</v>
+      </c>
+      <c r="H4" s="6">
+        <f>Mid!H4-'Mid to upper lower'!H4</f>
+        <v>0.65</v>
+      </c>
+      <c r="I4" s="6">
+        <f>Mid!I4-'Mid to upper lower'!I4</f>
+        <v>0.6</v>
+      </c>
+      <c r="J4" s="6">
+        <f>Mid!J4-'Mid to upper lower'!J4</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6">
+        <f>Mid!E5-'Mid to upper lower'!E5</f>
+        <v>0.97</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6">
+        <f>Mid!G5-'Mid to upper lower'!G5</f>
+        <v>0.95</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6">
+        <f>Mid!I5-'Mid to upper lower'!I5</f>
+        <v>0.96</v>
+      </c>
+      <c r="J5" s="6">
+        <f>Mid!J5-'Mid to upper lower'!J5</f>
+        <v>0.97</v>
+      </c>
+      <c r="K5" s="6">
+        <f>Mid!K5-'Mid to upper lower'!K5</f>
+        <v>0.98999999999999988</v>
+      </c>
+      <c r="L5" s="6">
+        <f>Mid!L5-'Mid to upper lower'!L5</f>
+        <v>1.01</v>
+      </c>
+      <c r="M5" s="6">
+        <f>Mid!M5-'Mid to upper lower'!M5</f>
+        <v>1.03</v>
+      </c>
+      <c r="N5" s="6">
+        <f>Mid!N5-'Mid to upper lower'!N5</f>
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6">
+        <f>Mid!D6-'Mid to upper lower'!D6</f>
+        <v>0.92499999999999993</v>
+      </c>
+      <c r="E6" s="6">
+        <f>Mid!E6-'Mid to upper lower'!E6</f>
+        <v>0.9</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6">
+        <f>Mid!G6-'Mid to upper lower'!G6</f>
+        <v>0.84000000000000008</v>
+      </c>
+      <c r="H6" s="6">
+        <f>Mid!H6-'Mid to upper lower'!H6</f>
+        <v>0.8</v>
+      </c>
+      <c r="I6" s="6">
+        <f>Mid!I6-'Mid to upper lower'!I6</f>
+        <v>0.74</v>
+      </c>
+      <c r="J6" s="6">
+        <f>Mid!J6-'Mid to upper lower'!J6</f>
+        <v>0.7</v>
+      </c>
+      <c r="K6" s="6">
+        <f>Mid!K6-'Mid to upper lower'!K6</f>
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="L6" s="6">
+        <f>Mid!L6-'Mid to upper lower'!L6</f>
+        <v>0.65</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6">
+        <f>Mid!C7-'Mid to upper lower'!C7</f>
+        <v>0.91999999999999993</v>
+      </c>
+      <c r="D7" s="6">
+        <f>Mid!D7-'Mid to upper lower'!D7</f>
+        <v>0.99</v>
+      </c>
+      <c r="E7" s="6">
+        <f>Mid!E7-'Mid to upper lower'!E7</f>
+        <v>1.23</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6">
+        <f>Mid!G7-'Mid to upper lower'!G7</f>
+        <v>1.35</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <f>Mid!B8-'Mid to upper lower'!B8</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <f>Mid!C8-'Mid to upper lower'!C8</f>
+        <v>0.97</v>
+      </c>
+      <c r="D8" s="6">
+        <f>Mid!D8-'Mid to upper lower'!D8</f>
+        <v>0.93499999999999994</v>
+      </c>
+      <c r="E8" s="6">
+        <f>Mid!E8-'Mid to upper lower'!E8</f>
+        <v>0.88</v>
+      </c>
+      <c r="F8" s="6">
+        <f>Mid!F8-'Mid to upper lower'!F8</f>
+        <v>0.85</v>
+      </c>
+      <c r="G8" s="6">
+        <f>Mid!G8-'Mid to upper lower'!G8</f>
+        <v>0.82</v>
+      </c>
+      <c r="H8" s="6">
+        <f>Mid!H8-'Mid to upper lower'!H8</f>
+        <v>0.80499999999999994</v>
+      </c>
+      <c r="I8" s="6">
+        <f>Mid!I8-'Mid to upper lower'!I8</f>
+        <v>0.78999999999999992</v>
+      </c>
+      <c r="J8" s="6">
+        <f>Mid!J8-'Mid to upper lower'!J8</f>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="K8" s="6">
+        <f>Mid!K8-'Mid to upper lower'!K8</f>
+        <v>0.77</v>
+      </c>
+      <c r="L8" s="6">
+        <f>Mid!L8-'Mid to upper lower'!L8</f>
+        <v>0.76</v>
+      </c>
+      <c r="M8" s="6">
+        <f>Mid!M8-'Mid to upper lower'!M8</f>
+        <v>0.76</v>
+      </c>
+      <c r="N8" s="6">
+        <f>Mid!N8-'Mid to upper lower'!N8</f>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6">
+        <f>Mid!C9-'Mid to upper lower'!C9</f>
+        <v>0.82</v>
+      </c>
+      <c r="D9" s="6">
+        <f>Mid!D9-'Mid to upper lower'!D9</f>
+        <v>0.82</v>
+      </c>
+      <c r="E9" s="6">
+        <f>Mid!E9-'Mid to upper lower'!E9</f>
+        <v>0.82000000000000006</v>
+      </c>
+      <c r="F9" s="6">
+        <f>Mid!F9-'Mid to upper lower'!F9</f>
+        <v>0.83</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6">
+        <f>Mid!D10-'Mid to upper lower'!D10</f>
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="E10" s="6">
+        <f>Mid!E10-'Mid to upper lower'!E10</f>
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="F10" s="6">
+        <f>Mid!F10-'Mid to upper lower'!F10</f>
+        <v>0.79499999999999993</v>
+      </c>
+      <c r="G10" s="6">
+        <f>Mid!G10-'Mid to upper lower'!G10</f>
+        <v>0.75</v>
+      </c>
+      <c r="H10" s="6">
+        <f>Mid!H10-'Mid to upper lower'!H10</f>
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="I10" s="6">
+        <f>Mid!I10-'Mid to upper lower'!I10</f>
+        <v>0.72</v>
+      </c>
+      <c r="J10" s="6">
+        <f>Mid!J10-'Mid to upper lower'!J10</f>
+        <v>0.71</v>
+      </c>
+      <c r="K10" s="6">
+        <f>Mid!K10-'Mid to upper lower'!K10</f>
+        <v>0.71</v>
+      </c>
+      <c r="L10" s="6">
+        <f>Mid!L10-'Mid to upper lower'!L10</f>
+        <v>0.69</v>
+      </c>
+      <c r="M10" s="6">
+        <f>Mid!M10-'Mid to upper lower'!M10</f>
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="N10" s="6">
+        <f>Mid!N10-'Mid to upper lower'!N10</f>
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6">
+        <f>Mid!E11-'Mid to upper lower'!E11</f>
+        <v>0.85</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6">
+        <f>Mid!G11-'Mid to upper lower'!G11</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6">
+        <f>Mid!I11-'Mid to upper lower'!I11</f>
+        <v>0.6</v>
+      </c>
+      <c r="J11" s="6">
+        <f>Mid!J11-'Mid to upper lower'!J11</f>
+        <v>0.52</v>
+      </c>
+      <c r="K11" s="6">
+        <f>Mid!K11-'Mid to upper lower'!K11</f>
+        <v>0.45999999999999996</v>
+      </c>
+      <c r="L11" s="6">
+        <f>Mid!L11-'Mid to upper lower'!L11</f>
+        <v>0.42</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6">
+        <f>Mid!D12-'Mid to upper lower'!D12</f>
+        <v>0.86</v>
+      </c>
+      <c r="E12" s="6">
+        <f>Mid!E12-'Mid to upper lower'!E12</f>
+        <v>0.78</v>
+      </c>
+      <c r="F12" s="6">
+        <f>Mid!F12-'Mid to upper lower'!F12</f>
+        <v>0.73</v>
+      </c>
+      <c r="G12" s="6">
+        <f>Mid!G12-'Mid to upper lower'!G12</f>
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="H12" s="6">
+        <f>Mid!H12-'Mid to upper lower'!H12</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="I12" s="6">
+        <f>Mid!I12-'Mid to upper lower'!I12</f>
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="J12" s="6">
+        <f>Mid!J12-'Mid to upper lower'!J12</f>
+        <v>0.64</v>
+      </c>
+      <c r="K12" s="6">
+        <f>Mid!K12-'Mid to upper lower'!K12</f>
+        <v>0.62</v>
+      </c>
+      <c r="L12" s="6">
+        <f>Mid!L12-'Mid to upper lower'!L12</f>
+        <v>0.68</v>
+      </c>
+      <c r="M12" s="6">
+        <f>Mid!M12-'Mid to upper lower'!M12</f>
+        <v>0.66</v>
+      </c>
+      <c r="N12" s="6">
+        <f>Mid!N12-'Mid to upper lower'!N12</f>
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6">
+        <f>Mid!D13-'Mid to upper lower'!D13</f>
+        <v>0.87999999999999989</v>
+      </c>
+      <c r="E13" s="6">
+        <f>Mid!E13-'Mid to upper lower'!E13</f>
+        <v>0.90999999999999992</v>
+      </c>
+      <c r="F13" s="6">
+        <f>Mid!F13-'Mid to upper lower'!F13</f>
+        <v>0.93</v>
+      </c>
+      <c r="G13" s="6">
+        <f>Mid!G13-'Mid to upper lower'!G13</f>
+        <v>0.96000000000000008</v>
+      </c>
+      <c r="H13" s="6">
+        <f>Mid!H13-'Mid to upper lower'!H13</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="I13" s="6">
+        <f>Mid!I13-'Mid to upper lower'!I13</f>
+        <v>1.05</v>
+      </c>
+      <c r="J13" s="6">
+        <f>Mid!J13-'Mid to upper lower'!J13</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K13" s="6">
+        <f>Mid!K13-'Mid to upper lower'!K13</f>
+        <v>1.26</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <f>Mid!B14-'Mid to upper lower'!B14</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
+        <f>Mid!C14-'Mid to upper lower'!C14</f>
+        <v>0.95</v>
+      </c>
+      <c r="D14" s="6">
+        <f>Mid!D14-'Mid to upper lower'!D14</f>
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="6">
+        <f>Mid!E14-'Mid to upper lower'!E14</f>
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <f>Mid!B15-'Mid to upper lower'!B15</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="6">
+        <f>Mid!C15-'Mid to upper lower'!C15</f>
+        <v>0.99500000000000011</v>
+      </c>
+      <c r="D15" s="6">
+        <f>Mid!D15-'Mid to upper lower'!D15</f>
+        <v>0.98999999999999988</v>
+      </c>
+      <c r="E15" s="6">
+        <f>Mid!E15-'Mid to upper lower'!E15</f>
+        <v>0.98</v>
+      </c>
+      <c r="F15" s="6">
+        <f>Mid!F15-'Mid to upper lower'!F15</f>
+        <v>0.98999999999999988</v>
+      </c>
+      <c r="G15" s="6">
+        <f>Mid!G15-'Mid to upper lower'!G15</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="6">
+        <f>Mid!H15-'Mid to upper lower'!H15</f>
+        <v>1.0050000000000001</v>
+      </c>
+      <c r="I15" s="6">
+        <f>Mid!I15-'Mid to upper lower'!I15</f>
+        <v>1.01</v>
+      </c>
+      <c r="J15" s="6">
+        <f>Mid!J15-'Mid to upper lower'!J15</f>
+        <v>1.02</v>
+      </c>
+      <c r="K15" s="6">
+        <f>Mid!K15-'Mid to upper lower'!K15</f>
+        <v>1.03</v>
+      </c>
+      <c r="L15" s="6">
+        <f>Mid!L15-'Mid to upper lower'!L15</f>
+        <v>1.0399999999999998</v>
+      </c>
+      <c r="M15" s="6">
+        <f>Mid!M15-'Mid to upper lower'!M15</f>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="N15" s="6">
+        <f>Mid!N15-'Mid to upper lower'!N15</f>
+        <v>1.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3586D6C1-6F84-0840-BC32-5B3BC0B00A73}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8">
+        <v>25</v>
+      </c>
+      <c r="D1" s="8">
+        <v>50</v>
+      </c>
+      <c r="E1" s="8">
+        <v>100</v>
+      </c>
+      <c r="F1" s="8">
+        <v>150</v>
+      </c>
+      <c r="G1" s="8">
+        <v>200</v>
+      </c>
+      <c r="H1" s="8">
+        <v>250</v>
+      </c>
+      <c r="I1" s="8">
+        <v>300</v>
+      </c>
+      <c r="J1" s="8">
+        <v>400</v>
+      </c>
+      <c r="K1" s="8">
+        <v>500</v>
+      </c>
+      <c r="L1" s="8">
+        <v>600</v>
+      </c>
+      <c r="M1" s="8">
+        <v>700</v>
+      </c>
+      <c r="N1" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="F2" s="10">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="H2" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0.17</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0.32</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="L3" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+    </row>
+    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0.45</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="K5" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="M5" s="10">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0.16</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="E7" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="H8" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="J8" s="10">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="L8" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="N8" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E10" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="L10" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="M10" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N10" s="10">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="K11" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="L12" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="M12" s="10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N12" s="10">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="E13" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.16</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0.19</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0.31</v>
+      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+    </row>
+    <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+    </row>
+    <row r="15" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="D15" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="10">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="H15" s="10">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="I15" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="K15" s="10">
+        <v>0.09</v>
+      </c>
+      <c r="L15" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="M15" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="N15" s="10">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correction of a legumes RR value in upper UI
</commit_message>
<xml_diff>
--- a/data/RR_table_quanti.xlsx
+++ b/data/RR_table_quanti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inesmasurel/Library/Mobile Documents/com~apple~CloudDocs/Desktop/Pasteur-Cnam/Stage MS - ENS/DOUGLAS/DOUGLAS_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2431A3-9236-4E49-A1EA-A69E164CB583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DAF257-E4CD-3B43-B7FA-6DB72BC92D4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mid" sheetId="1" r:id="rId1"/>
@@ -89,23 +89,27 @@
       <sz val="11"/>
       <color rgb="FF262626"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -398,7 +402,7 @@
   <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -935,7 +939,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1038,7 +1042,7 @@
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1089,7 +1093,7 @@
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1391,10 +1395,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="6">
-        <f>Mid!C11+'Mid to upper lower'!C11</f>
-        <v>1.4999999999999999E-2</v>
-      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6">
         <f>Mid!E11+'Mid to upper lower'!E11</f>
@@ -1425,7 +1426,7 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1476,7 +1477,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -1518,7 +1519,7 @@
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
     </row>
-    <row r="14" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -1548,7 +1549,7 @@
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
     </row>
-    <row r="15" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -2102,7 +2103,7 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -2225,7 +2226,7 @@
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
     </row>
-    <row r="15" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -2292,7 +2293,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
RR mid to upper/lower when intake=0 always equals to 0. Rebuilt the initial RR tbale and the linear interpolation RR tables
</commit_message>
<xml_diff>
--- a/data/RR_table_quanti.xlsx
+++ b/data/RR_table_quanti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inesmasurel/Library/Mobile Documents/com~apple~CloudDocs/Desktop/Pasteur-Cnam/Stage MS - ENS/DOUGLAS/DOUGLAS_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DAF257-E4CD-3B43-B7FA-6DB72BC92D4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A757FAD-265B-DC46-A68B-2E0052E99E3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mid" sheetId="1" r:id="rId1"/>
@@ -159,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -180,7 +180,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52511AF-CE91-C645-B98F-638F567A8977}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1142,7 +1141,10 @@
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6">
+        <f>Mid!B5+'Mid to upper lower'!B5</f>
+        <v>1</v>
+      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6">
@@ -1184,7 +1186,10 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6">
+        <f>Mid!B6+'Mid to upper lower'!B6</f>
+        <v>1</v>
+      </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6">
         <f>Mid!D6+'Mid to upper lower'!D6</f>
@@ -1226,7 +1231,10 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6">
+        <f>Mid!B7+'Mid to upper lower'!B7</f>
+        <v>1</v>
+      </c>
       <c r="C7" s="6">
         <f>Mid!C7+'Mid to upper lower'!C7</f>
         <v>1.04</v>
@@ -1313,7 +1321,10 @@
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="6">
+        <f>Mid!B9+'Mid to upper lower'!B9</f>
+        <v>1</v>
+      </c>
       <c r="C9" s="6">
         <f>Mid!C9+'Mid to upper lower'!C9</f>
         <v>0.86</v>
@@ -1343,7 +1354,10 @@
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="6">
+        <f>Mid!B10+'Mid to upper lower'!B10</f>
+        <v>1</v>
+      </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6">
         <f>Mid!D10+'Mid to upper lower'!D10</f>
@@ -1394,7 +1408,10 @@
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="6">
+        <f>Mid!B11+'Mid to upper lower'!B11</f>
+        <v>1</v>
+      </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6">
@@ -1430,7 +1447,10 @@
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="6">
+        <f>Mid!B12+'Mid to upper lower'!B12</f>
+        <v>1</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6">
         <f>Mid!D12+'Mid to upper lower'!D12</f>
@@ -1481,7 +1501,10 @@
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="6">
+        <f>Mid!B13+'Mid to upper lower'!B13</f>
+        <v>1</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6">
         <f>Mid!D13+'Mid to upper lower'!D13</f>
@@ -1615,8 +1638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A723EE2E-8835-E04A-880B-B880DB74E2B3}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1819,7 +1842,10 @@
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6">
+        <f>Mid!B5-'Mid to upper lower'!B5</f>
+        <v>1</v>
+      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6">
@@ -1861,7 +1887,10 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6">
+        <f>Mid!B6-'Mid to upper lower'!B6</f>
+        <v>1</v>
+      </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6">
         <f>Mid!D6-'Mid to upper lower'!D6</f>
@@ -1903,7 +1932,10 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6">
+        <f>Mid!B7-'Mid to upper lower'!B7</f>
+        <v>1</v>
+      </c>
       <c r="C7" s="6">
         <f>Mid!C7-'Mid to upper lower'!C7</f>
         <v>0.91999999999999993</v>
@@ -1990,7 +2022,10 @@
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="6">
+        <f>Mid!B9-'Mid to upper lower'!B9</f>
+        <v>1</v>
+      </c>
       <c r="C9" s="6">
         <f>Mid!C9-'Mid to upper lower'!C9</f>
         <v>0.82</v>
@@ -2020,7 +2055,10 @@
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="6">
+        <f>Mid!B10-'Mid to upper lower'!B10</f>
+        <v>1</v>
+      </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6">
         <f>Mid!D10-'Mid to upper lower'!D10</f>
@@ -2071,7 +2109,10 @@
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="6">
+        <f>Mid!B11-'Mid to upper lower'!B11</f>
+        <v>1</v>
+      </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6">
@@ -2107,7 +2148,10 @@
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="6">
+        <f>Mid!B12-'Mid to upper lower'!B12</f>
+        <v>1</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6">
         <f>Mid!D12-'Mid to upper lower'!D12</f>
@@ -2158,7 +2202,10 @@
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="6">
+        <f>Mid!B13-'Mid to upper lower'!B13</f>
+        <v>1</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6">
         <f>Mid!D13-'Mid to upper lower'!D13</f>
@@ -2293,7 +2340,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2465,7 +2512,9 @@
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
       <c r="C5" s="10">
         <v>0.01</v>
       </c>
@@ -2507,7 +2556,9 @@
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
       <c r="C6" s="10">
         <v>0.02</v>
       </c>
@@ -2545,7 +2596,9 @@
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
       <c r="C7" s="10">
         <v>0.06</v>
       </c>
@@ -2617,7 +2670,9 @@
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
       <c r="C9" s="10">
         <v>0.02</v>
       </c>
@@ -2643,7 +2698,9 @@
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10">
         <v>1.4999999999999999E-2</v>
@@ -2683,7 +2740,9 @@
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
       <c r="C11" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -2721,7 +2780,9 @@
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="10"/>
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10">
         <v>0.01</v>
@@ -2761,7 +2822,9 @@
       <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="12"/>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
       <c r="C13" s="10">
         <v>0.03</v>
       </c>

</xml_diff>